<commit_message>
Persistance dans le serveur
</commit_message>
<xml_diff>
--- a/parent-project-jeumemoire/persistancejeumemory-v0/jeumemory_bdd/BDD.xlsx
+++ b/parent-project-jeumemoire/persistancejeumemory-v0/jeumemory_bdd/BDD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\Workspace-Projet-DAO\Ressources-Tp-DAO (1)\CarnetAdressesDAO\carnetadr_bdd\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>IdJoueur</t>
   </si>
@@ -84,12 +84,91 @@
   </si>
   <si>
     <t>nbPair</t>
+  </si>
+  <si>
+    <t>leclerc</t>
+  </si>
+  <si>
+    <t>jacques</t>
+  </si>
+  <si>
+    <t>jac</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>jojo</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>jjs</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>zb</t>
+  </si>
+  <si>
+    <t>uy</t>
+  </si>
+  <si>
+    <t>njk</t>
+  </si>
+  <si>
+    <t>mgu</t>
+  </si>
+  <si>
+    <t>kjnj</t>
+  </si>
+  <si>
+    <t>vuy</t>
+  </si>
+  <si>
+    <t>jkb</t>
+  </si>
+  <si>
+    <t>kjjb</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>eth</t>
+  </si>
+  <si>
+    <t>rjjy</t>
+  </si>
+  <si>
+    <t>ver</t>
+  </si>
+  <si>
+    <t>umy</t>
+  </si>
+  <si>
+    <t>rhser</t>
+  </si>
+  <si>
+    <t>obtrs</t>
+  </si>
+  <si>
+    <t>vbiau</t>
+  </si>
+  <si>
+    <t>cevwg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -469,6 +548,176 @@
       </c>
       <c r="E3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>